<commit_message>
Added an extra array formulae test
</commit_message>
<xml_diff>
--- a/examples/arrayformulatest.xlsx
+++ b/examples/arrayformulatest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="260" windowWidth="25360" windowHeight="17240" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Referencing" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
   <dimension ref="C3:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -909,6 +909,9 @@
       <c r="G22">
         <v>137.26515207025273</v>
       </c>
+      <c r="L22">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" spans="3:15">
       <c r="D23" t="s">
@@ -917,6 +920,9 @@
       <c r="G23">
         <v>30.731004194832696</v>
       </c>
+      <c r="L23">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="3:15">
       <c r="D24" t="s">
@@ -925,6 +931,9 @@
       <c r="G24">
         <v>20.487336129888465</v>
       </c>
+      <c r="L24">
+        <v>3</v>
+      </c>
     </row>
     <row r="25" spans="3:15">
       <c r="D25" t="s">
@@ -933,6 +942,9 @@
       <c r="G25">
         <v>8.1949344519553868</v>
       </c>
+      <c r="L25">
+        <v>-1</v>
+      </c>
     </row>
     <row r="26" spans="3:15">
       <c r="D26" t="s">
@@ -940,6 +952,10 @@
       </c>
       <c r="G26">
         <v>8.1949344519553868</v>
+      </c>
+      <c r="L26">
+        <f t="array" ref="L26">AVERAGE(IF(L22:L25&gt;0,L22:L25,""))</f>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="3:15">

</xml_diff>